<commit_message>
Added an X for closed pop review
</commit_message>
<xml_diff>
--- a/ChaptersHandling.xlsx
+++ b/ChaptersHandling.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="16275" windowHeight="6975"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>Chapter</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>When you review a final draft, just put an X under your name in that row and we can easily see what is completely done, edited, and reviewed.</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -482,7 +485,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,6 +581,9 @@
       </c>
       <c r="D7" t="s">
         <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final draft of Ch10 now available
</commit_message>
<xml_diff>
--- a/ChaptersHandling.xlsx
+++ b/ChaptersHandling.xlsx
@@ -485,7 +485,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,7 +664,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
         <v>30</v>

</xml_diff>